<commit_message>
Added child deletion flow
</commit_message>
<xml_diff>
--- a/src/main/resources/static/UploadChildrenTemplate.xlsx
+++ b/src/main/resources/static/UploadChildrenTemplate.xlsx
@@ -38,9 +38,6 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>Aspiration</t>
-  </si>
-  <si>
     <t>Image Name</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>test2.jpg</t>
+  </si>
+  <si>
+    <t>Aspirations</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,18 +399,18 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>2000</v>
@@ -419,18 +419,18 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>2008</v>
@@ -439,10 +439,10 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring- moved logic in controller to services, renamed desired_occupation column to information, rearranged files and endpoints
</commit_message>
<xml_diff>
--- a/src/main/resources/static/UploadChildrenTemplate.xlsx
+++ b/src/main/resources/static/UploadChildrenTemplate.xlsx
@@ -59,7 +59,7 @@
     <t>test2.jpg</t>
   </si>
   <si>
-    <t>Aspirations</t>
+    <t>Information</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>